<commit_message>
Template changes per redmine 35095
</commit_message>
<xml_diff>
--- a/Load/ontology/script/raw_detection_template.xlsx
+++ b/Load/ontology/script/raw_detection_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jjudkins/Documents/GitHub/ApiCommonData/Load/ontology/script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8FFFF7-F205-534E-B9E6-FB7AF706EE94}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F6BCF1-0E73-2540-A9CD-B63D2489197F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="72">
   <si>
     <t>variable</t>
   </si>
@@ -250,6 +250,15 @@
   </si>
   <si>
     <t>(loop-mediated thermal amplification)</t>
+  </si>
+  <si>
+    <t>ontological label</t>
+  </si>
+  <si>
+    <t>subclass axiom</t>
+  </si>
+  <si>
+    <t>subclass</t>
   </si>
 </sst>
 </file>
@@ -1102,13 +1111,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T15"/>
+  <dimension ref="A1:V15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N3" sqref="N3"/>
+      <selection pane="bottomRight" activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1127,11 +1136,14 @@
     <col min="12" max="12" width="22.6640625" style="1" customWidth="1"/>
     <col min="13" max="13" width="23.33203125" style="1" customWidth="1"/>
     <col min="14" max="14" width="30.33203125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="18.33203125" style="2" customWidth="1"/>
-    <col min="16" max="16384" width="10.83203125" style="1"/>
+    <col min="15" max="16" width="18.33203125" style="2" customWidth="1"/>
+    <col min="17" max="17" width="17.1640625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="10.83203125" style="2"/>
+    <col min="19" max="20" width="15.5" style="2" customWidth="1"/>
+    <col min="21" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1174,8 +1186,17 @@
       <c r="O1" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="T1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>70</v>
+      </c>
     </row>
-    <row r="2" spans="1:20" ht="102" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" ht="102" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>28</v>
       </c>
@@ -1204,7 +1225,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="125" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" ht="125" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
@@ -1235,14 +1256,14 @@
         <f>TRIM("Raw "&amp;LOWER($E3)&amp;" data for "&amp;$B3)</f>
         <v>Raw bacteria data for stool</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="Q3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="R3" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>46</v>
       </c>
@@ -1274,14 +1295,14 @@
         <f t="shared" ref="O4:O12" si="1">TRIM("Raw "&amp;LOWER($E4)&amp;" data for "&amp;$B4)</f>
         <v>Raw virus data for blood</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="Q4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="R4" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" ht="34" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>29</v>
       </c>
@@ -1308,14 +1329,14 @@
         <f t="shared" si="1"/>
         <v>Raw bacteria data for urine</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="Q5" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="R5" s="1" t="s">
+      <c r="R5" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="34" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" ht="34" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>29</v>
       </c>
@@ -1342,11 +1363,11 @@
         <f t="shared" si="1"/>
         <v>Raw eukaryota data for urine</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="Q6" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
@@ -1370,11 +1391,11 @@
         <f t="shared" si="1"/>
         <v>Raw bacteria data for stool</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="Q7" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
@@ -1401,14 +1422,14 @@
         <f t="shared" si="1"/>
         <v>Raw virus data for stool</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="Q8" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="R8" s="1" t="s">
+      <c r="R8" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" ht="64" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1435,14 +1456,14 @@
         <f t="shared" si="1"/>
         <v>Raw virus data for stool</v>
       </c>
-      <c r="Q9" s="1" t="s">
+      <c r="Q9" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="T9" s="1" t="s">
+      <c r="S9" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="67" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" ht="67" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
@@ -1475,11 +1496,11 @@
         <f t="shared" si="1"/>
         <v>Raw bacteria data for stool</v>
       </c>
-      <c r="Q10" s="1" t="s">
+      <c r="Q10" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22" ht="34" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>12</v>
       </c>
@@ -1512,11 +1533,11 @@
         <f t="shared" si="1"/>
         <v>Raw bacteria data for stool</v>
       </c>
-      <c r="Q11" s="1" t="s">
+      <c r="Q11" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" ht="51" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
@@ -1543,25 +1564,25 @@
         <f t="shared" si="1"/>
         <v>Raw bacteria data for stool</v>
       </c>
-      <c r="Q12" s="1" t="s">
+      <c r="Q12" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="T12" s="1" t="s">
+      <c r="S12" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="Q13" s="1" t="s">
+    <row r="13" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q13" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="Q14" s="1" t="s">
+    <row r="14" spans="1:22" ht="34" x14ac:dyDescent="0.2">
+      <c r="Q14" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="Q15" s="1" t="s">
+    <row r="15" spans="1:22" ht="34" x14ac:dyDescent="0.2">
+      <c r="Q15" s="2" t="s">
         <v>65</v>
       </c>
     </row>

</xml_diff>